<commit_message>
Update to multiclock branch (Many more bugfixes and output file tweaks, ported changes to VTR_flow from trunk, new testing framework with expanded QoR parsing)
</commit_message>
<xml_diff>
--- a/multiclock/vtr_flow/tasks/molecule_timing_small/molecule_timing_small_comparison.xlsx
+++ b/multiclock/vtr_flow/tasks/molecule_timing_small/molecule_timing_small_comparison.xlsx
@@ -454,7 +454,7 @@
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -552,27 +552,27 @@
       </c>
       <c r="D2" s="2">
         <f>'molecule timing small'!D2/'6.0'!D2</f>
-        <v>0.77083333333333337</v>
+        <v>0.9375</v>
       </c>
       <c r="E2" s="2">
         <f>'molecule timing small'!E2/'6.0'!E2</f>
-        <v>1.0231232049642565</v>
+        <v>0.9896787628491367</v>
       </c>
       <c r="F2" s="2">
         <f>'molecule timing small'!F2/'6.0'!F2</f>
-        <v>0.31328917901558107</v>
+        <v>0.96504185130477593</v>
       </c>
       <c r="G2" s="2">
         <f>'molecule timing small'!G2/'6.0'!G2</f>
-        <v>0.91208884367582244</v>
+        <v>2.043743641912513</v>
       </c>
       <c r="H2" s="2">
         <f>'molecule timing small'!H2/'6.0'!H2</f>
-        <v>0.37497301964170082</v>
+        <v>2.2600097129289876</v>
       </c>
       <c r="I2" s="2">
         <f>'molecule timing small'!I2/'6.0'!I2</f>
-        <v>0.58850931677018625</v>
+        <v>1.4472049689440993</v>
       </c>
       <c r="J2" s="2">
         <f>'molecule timing small'!J2/'6.0'!J2</f>
@@ -584,7 +584,7 @@
       </c>
       <c r="L2" s="2">
         <f>'molecule timing small'!L2/'6.0'!L2</f>
-        <v>0.85786945464820574</v>
+        <v>1.0110200621644532</v>
       </c>
       <c r="M2" s="2">
         <f>'molecule timing small'!M2/'6.0'!M2</f>
@@ -634,23 +634,23 @@
       </c>
       <c r="E3" s="2">
         <f>'molecule timing small'!E3/'6.0'!E3</f>
-        <v>1.0088563127414898</v>
+        <v>0.99095252497875619</v>
       </c>
       <c r="F3" s="2">
         <f>'molecule timing small'!F3/'6.0'!F3</f>
-        <v>0.35039852851011649</v>
+        <v>0.9367910790925813</v>
       </c>
       <c r="G3" s="2">
         <f>'molecule timing small'!G3/'6.0'!G3</f>
-        <v>0.93885068762278978</v>
+        <v>1.7718565815324168</v>
       </c>
       <c r="H3" s="2">
         <f>'molecule timing small'!H3/'6.0'!H3</f>
-        <v>0.77390823659480379</v>
+        <v>0.87866224433388607</v>
       </c>
       <c r="I3" s="2">
         <f>'molecule timing small'!I3/'6.0'!I3</f>
-        <v>0.88888888888888895</v>
+        <v>1.3006535947712419</v>
       </c>
       <c r="J3" s="2">
         <f>'molecule timing small'!J3/'6.0'!J3</f>
@@ -662,11 +662,11 @@
       </c>
       <c r="L3" s="2">
         <f>'molecule timing small'!L3/'6.0'!L3</f>
-        <v>0.91663310511478047</v>
+        <v>0.95489327426500203</v>
       </c>
       <c r="M3" s="2">
         <f>'molecule timing small'!M3/'6.0'!M3</f>
-        <v>1.0177777777777777</v>
+        <v>1.0088888888888889</v>
       </c>
       <c r="N3" s="2">
         <f>'molecule timing small'!N3/'6.0'!N3</f>
@@ -708,27 +708,27 @@
       </c>
       <c r="D4" s="2">
         <f>'molecule timing small'!D4/'6.0'!D4</f>
-        <v>1.125</v>
+        <v>1.0416666666666667</v>
       </c>
       <c r="E4" s="2">
         <f>'molecule timing small'!E4/'6.0'!E4</f>
-        <v>0.92499591337407661</v>
+        <v>0.90696993825240069</v>
       </c>
       <c r="F4" s="2">
         <f>'molecule timing small'!F4/'6.0'!F4</f>
-        <v>0.81188310431585065</v>
+        <v>3.1107025353203017</v>
       </c>
       <c r="G4" s="2">
         <f>'molecule timing small'!G4/'6.0'!G4</f>
-        <v>0.91830985915492958</v>
+        <v>1.8084507042253521</v>
       </c>
       <c r="H4" s="2">
         <f>'molecule timing small'!H4/'6.0'!H4</f>
-        <v>1.0101010101010102</v>
+        <v>2.5505050505050506</v>
       </c>
       <c r="I4" s="2">
         <f>'molecule timing small'!I4/'6.0'!I4</f>
-        <v>1</v>
+        <v>1.8235294117647058</v>
       </c>
       <c r="J4" s="2">
         <f>'molecule timing small'!J4/'6.0'!J4</f>
@@ -740,7 +740,7 @@
       </c>
       <c r="L4" s="2">
         <f>'molecule timing small'!L4/'6.0'!L4</f>
-        <v>0.95327102803738317</v>
+        <v>1.0420560747663552</v>
       </c>
       <c r="M4" s="2">
         <f>'molecule timing small'!M4/'6.0'!M4</f>
@@ -786,27 +786,27 @@
       </c>
       <c r="D5" s="2">
         <f>'molecule timing small'!D5/'6.0'!D5</f>
-        <v>1</v>
+        <v>0.96875</v>
       </c>
       <c r="E5" s="2">
         <f>'molecule timing small'!E5/'6.0'!E5</f>
-        <v>1.0161145550650619</v>
+        <v>1.0089391163764823</v>
       </c>
       <c r="F5" s="2">
         <f>'molecule timing small'!F5/'6.0'!F5</f>
-        <v>0.19016659894351889</v>
+        <v>0.53596099146688336</v>
       </c>
       <c r="G5" s="2">
         <f>'molecule timing small'!G5/'6.0'!G5</f>
-        <v>0.95744680851063824</v>
+        <v>1.7872340425531914</v>
       </c>
       <c r="H5" s="2">
         <f>'molecule timing small'!H5/'6.0'!H5</f>
-        <v>1.0674157303370786</v>
+        <v>1.9130691898285039</v>
       </c>
       <c r="I5" s="2">
         <f>'molecule timing small'!I5/'6.0'!I5</f>
-        <v>0.81889763779527558</v>
+        <v>1.3700787401574803</v>
       </c>
       <c r="J5" s="2">
         <f>'molecule timing small'!J5/'6.0'!J5</f>
@@ -818,7 +818,7 @@
       </c>
       <c r="L5" s="2">
         <f>'molecule timing small'!L5/'6.0'!L5</f>
-        <v>0.9971949509116409</v>
+        <v>0.99579242636746146</v>
       </c>
       <c r="M5" s="2">
         <f>'molecule timing small'!M5/'6.0'!M5</f>
@@ -864,27 +864,27 @@
       </c>
       <c r="D6" s="2">
         <f>'molecule timing small'!D6/'6.0'!D6</f>
-        <v>1.0714285714285714</v>
+        <v>0.8928571428571429</v>
       </c>
       <c r="E6" s="2">
         <f>'molecule timing small'!E6/'6.0'!E6</f>
-        <v>0.95146006575130537</v>
+        <v>0.95923532824462221</v>
       </c>
       <c r="F6" s="2">
         <f>'molecule timing small'!F6/'6.0'!F6</f>
-        <v>1.4569017480409887</v>
+        <v>3.93128390596745</v>
       </c>
       <c r="G6" s="2">
         <f>'molecule timing small'!G6/'6.0'!G6</f>
-        <v>0.88652482269503552</v>
+        <v>1.7588652482269505</v>
       </c>
       <c r="H6" s="2">
         <f>'molecule timing small'!H6/'6.0'!H6</f>
-        <v>1.0284495021337128</v>
+        <v>1.2574679943100995</v>
       </c>
       <c r="I6" s="2">
         <f>'molecule timing small'!I6/'6.0'!I6</f>
-        <v>0.94736842105263164</v>
+        <v>1.8315789473684212</v>
       </c>
       <c r="J6" s="2">
         <f>'molecule timing small'!J6/'6.0'!J6</f>
@@ -896,7 +896,7 @@
       </c>
       <c r="L6" s="2">
         <f>'molecule timing small'!L6/'6.0'!L6</f>
-        <v>0.90528634361233484</v>
+        <v>0.92070484581497802</v>
       </c>
       <c r="M6" s="2">
         <f>'molecule timing small'!M6/'6.0'!M6</f>
@@ -942,27 +942,27 @@
       </c>
       <c r="D7" s="2">
         <f>'molecule timing small'!D7/'6.0'!D7</f>
-        <v>0.93617021276595747</v>
+        <v>0.97872340425531912</v>
       </c>
       <c r="E7" s="2">
         <f>'molecule timing small'!E7/'6.0'!E7</f>
-        <v>1.0593178535900927</v>
+        <v>1.0874222747165716</v>
       </c>
       <c r="F7" s="2">
         <f>'molecule timing small'!F7/'6.0'!F7</f>
-        <v>0.48111086940758463</v>
+        <v>1.1001649626568051</v>
       </c>
       <c r="G7" s="2">
         <f>'molecule timing small'!G7/'6.0'!G7</f>
-        <v>0.75311490539916937</v>
+        <v>1.4949568198299164</v>
       </c>
       <c r="H7" s="2">
         <f>'molecule timing small'!H7/'6.0'!H7</f>
-        <v>2.608367827411636</v>
+        <v>4.2393247880345299</v>
       </c>
       <c r="I7" s="2">
         <f>'molecule timing small'!I7/'6.0'!I7</f>
-        <v>0.69063180827886705</v>
+        <v>1.0254175744371823</v>
       </c>
       <c r="J7" s="2">
         <f>'molecule timing small'!J7/'6.0'!J7</f>
@@ -974,11 +974,11 @@
       </c>
       <c r="L7" s="2">
         <f>'molecule timing small'!L7/'6.0'!L7</f>
-        <v>0.93816442239546416</v>
+        <v>0.96350106307583272</v>
       </c>
       <c r="M7" s="2">
         <f>'molecule timing small'!M7/'6.0'!M7</f>
-        <v>0.96636771300448432</v>
+        <v>0.98206278026905824</v>
       </c>
       <c r="N7" s="2">
         <f>'molecule timing small'!N7/'6.0'!N7</f>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="D8" s="2">
         <f>'molecule timing small'!D8/'6.0'!D8</f>
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="E8" s="2">
         <f>'molecule timing small'!E8/'6.0'!E8</f>
@@ -1028,19 +1028,19 @@
       </c>
       <c r="F8" s="2">
         <f>'molecule timing small'!F8/'6.0'!F8</f>
-        <v>16.586897179253867</v>
+        <v>32.573248407643312</v>
       </c>
       <c r="G8" s="2">
         <f>'molecule timing small'!G8/'6.0'!G8</f>
-        <v>1.0311778290993072</v>
+        <v>1.9757505773672055</v>
       </c>
       <c r="H8" s="2">
         <f>'molecule timing small'!H8/'6.0'!H8</f>
-        <v>0.61297897320952077</v>
+        <v>0.81225317536556729</v>
       </c>
       <c r="I8" s="2">
         <f>'molecule timing small'!I8/'6.0'!I8</f>
-        <v>0.58213716108452951</v>
+        <v>0.84370015948963328</v>
       </c>
       <c r="J8" s="2">
         <f>'molecule timing small'!J8/'6.0'!J8</f>
@@ -1052,7 +1052,7 @@
       </c>
       <c r="L8" s="2">
         <f>'molecule timing small'!L8/'6.0'!L8</f>
-        <v>0.99593495934959353</v>
+        <v>0.99695121951219512</v>
       </c>
       <c r="M8" s="2">
         <f>'molecule timing small'!M8/'6.0'!M8</f>
@@ -1098,27 +1098,27 @@
       </c>
       <c r="D9" s="2">
         <f>'molecule timing small'!D9/'6.0'!D9</f>
-        <v>0.8571428571428571</v>
+        <v>0.94285714285714284</v>
       </c>
       <c r="E9" s="2">
         <f>'molecule timing small'!E9/'6.0'!E9</f>
-        <v>1.0304979706648476</v>
+        <v>1.0284594172476369</v>
       </c>
       <c r="F9" s="2">
         <f>'molecule timing small'!F9/'6.0'!F9</f>
-        <v>0.29739444813829791</v>
+        <v>0.6845495345744681</v>
       </c>
       <c r="G9" s="2">
         <f>'molecule timing small'!G9/'6.0'!G9</f>
-        <v>0.8990476190476191</v>
+        <v>1.7226666666666666</v>
       </c>
       <c r="H9" s="2">
         <f>'molecule timing small'!H9/'6.0'!H9</f>
-        <v>0.46738465304124344</v>
+        <v>0.97735895239260806</v>
       </c>
       <c r="I9" s="2">
         <f>'molecule timing small'!I9/'6.0'!I9</f>
-        <v>0.63861386138613863</v>
+        <v>1.2128712871287128</v>
       </c>
       <c r="J9" s="2">
         <f>'molecule timing small'!J9/'6.0'!J9</f>
@@ -1130,11 +1130,11 @@
       </c>
       <c r="L9" s="2">
         <f>'molecule timing small'!L9/'6.0'!L9</f>
-        <v>0.88149804359977646</v>
+        <v>0.92453884851872559</v>
       </c>
       <c r="M9" s="2">
         <f>'molecule timing small'!M9/'6.0'!M9</f>
-        <v>1.0253164556962024</v>
+        <v>1.0126582278481013</v>
       </c>
       <c r="N9" s="2">
         <f>'molecule timing small'!N9/'6.0'!N9</f>
@@ -1176,27 +1176,27 @@
       </c>
       <c r="D10" s="2">
         <f>'molecule timing small'!D10/'6.0'!D10</f>
-        <v>0.86363636363636365</v>
+        <v>0.95454545454545459</v>
       </c>
       <c r="E10" s="2">
         <f>'molecule timing small'!E10/'6.0'!E10</f>
-        <v>1.0194099996233505</v>
+        <v>0.99938062096932823</v>
       </c>
       <c r="F10" s="2">
         <f>'molecule timing small'!F10/'6.0'!F10</f>
-        <v>0.49348360217925435</v>
+        <v>1.1992041448563187</v>
       </c>
       <c r="G10" s="2">
         <f>'molecule timing small'!G10/'6.0'!G10</f>
-        <v>0.69781702232033349</v>
+        <v>1.3816531763551629</v>
       </c>
       <c r="H10" s="2">
         <f>'molecule timing small'!H10/'6.0'!H10</f>
-        <v>0.49643556480234979</v>
+        <v>0.82860115040998661</v>
       </c>
       <c r="I10" s="2">
         <f>'molecule timing small'!I10/'6.0'!I10</f>
-        <v>0.5714285714285714</v>
+        <v>1.0974789915966388</v>
       </c>
       <c r="J10" s="2">
         <f>'molecule timing small'!J10/'6.0'!J10</f>
@@ -1208,7 +1208,7 @@
       </c>
       <c r="L10" s="2">
         <f>'molecule timing small'!L10/'6.0'!L10</f>
-        <v>1.0007662835249043</v>
+        <v>1.0306513409961686</v>
       </c>
       <c r="M10" s="2">
         <f>'molecule timing small'!M10/'6.0'!M10</f>
@@ -1262,19 +1262,19 @@
       </c>
       <c r="F11" s="2">
         <f>'molecule timing small'!F11/'6.0'!F11</f>
-        <v>0.37402620999795588</v>
+        <v>1.1936905221558518</v>
       </c>
       <c r="G11" s="2">
         <f>'molecule timing small'!G11/'6.0'!G11</f>
-        <v>0.73099870298313885</v>
+        <v>1.412970168612192</v>
       </c>
       <c r="H11" s="2">
         <f>'molecule timing small'!H11/'6.0'!H11</f>
-        <v>0.79085457271364312</v>
+        <v>1.3713143428285857</v>
       </c>
       <c r="I11" s="2">
         <f>'molecule timing small'!I11/'6.0'!I11</f>
-        <v>0.8</v>
+        <v>1.3170731707317076</v>
       </c>
       <c r="J11" s="2">
         <f>'molecule timing small'!J11/'6.0'!J11</f>
@@ -1286,11 +1286,11 @@
       </c>
       <c r="L11" s="2">
         <f>'molecule timing small'!L11/'6.0'!L11</f>
-        <v>0.99185043144774687</v>
+        <v>1.0263662511984659</v>
       </c>
       <c r="M11" s="2">
         <f>'molecule timing small'!M11/'6.0'!M11</f>
-        <v>1.0238095238095237</v>
+        <v>1.0119047619047619</v>
       </c>
       <c r="N11" s="2">
         <f>'molecule timing small'!N11/'6.0'!N11</f>
@@ -1332,27 +1332,27 @@
       </c>
       <c r="D12" s="2">
         <f>'molecule timing small'!D12/'6.0'!D12</f>
-        <v>0.83870967741935487</v>
+        <v>1.032258064516129</v>
       </c>
       <c r="E12" s="2">
         <f>'molecule timing small'!E12/'6.0'!E12</f>
-        <v>1.0417345211865761</v>
+        <v>1.0286362039786698</v>
       </c>
       <c r="F12" s="2">
         <f>'molecule timing small'!F12/'6.0'!F12</f>
-        <v>0.24147732656193743</v>
+        <v>0.79996589035644572</v>
       </c>
       <c r="G12" s="2">
         <f>'molecule timing small'!G12/'6.0'!G12</f>
-        <v>0.74470588235294111</v>
+        <v>1.8423529411764705</v>
       </c>
       <c r="H12" s="2">
         <f>'molecule timing small'!H12/'6.0'!H12</f>
-        <v>0.3634635326650536</v>
+        <v>1.1723124783961285</v>
       </c>
       <c r="I12" s="2">
         <f>'molecule timing small'!I12/'6.0'!I12</f>
-        <v>0.64122137404580148</v>
+        <v>1.7862595419847327</v>
       </c>
       <c r="J12" s="2">
         <f>'molecule timing small'!J12/'6.0'!J12</f>
@@ -1364,11 +1364,11 @@
       </c>
       <c r="L12" s="2">
         <f>'molecule timing small'!L12/'6.0'!L12</f>
-        <v>0.68916155419222902</v>
+        <v>0.8880368098159509</v>
       </c>
       <c r="M12" s="2">
         <f>'molecule timing small'!M12/'6.0'!M12</f>
-        <v>1.0149253731343284</v>
+        <v>1.0099502487562189</v>
       </c>
       <c r="N12" s="2">
         <f>'molecule timing small'!N12/'6.0'!N12</f>
@@ -1563,27 +1563,27 @@
       </c>
       <c r="D22" s="2">
         <f>GEOMEAN(D2:D21)</f>
-        <v>0.9294423765740254</v>
+        <v>0.96325088847993556</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" ref="E22:O22" si="0">GEOMEAN(E2:E21)</f>
-        <v>1.0103822068063899</v>
+        <v>1.0032374591138487</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="0"/>
-        <v>0.58234208839147772</v>
+        <v>1.5919737959917484</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" si="0"/>
-        <v>0.85435981274180128</v>
+        <v>1.7146902769910179</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" si="0"/>
-        <v>0.73597290497108936</v>
+        <v>1.4386040961942979</v>
       </c>
       <c r="I22" s="2">
         <f t="shared" si="0"/>
-        <v>0.72822470827842911</v>
+        <v>1.3315772175172138</v>
       </c>
       <c r="J22" s="2">
         <f t="shared" si="0"/>
@@ -1595,11 +1595,11 @@
       </c>
       <c r="L22" s="2">
         <f t="shared" si="0"/>
-        <v>0.91607289370296296</v>
+        <v>0.97645842399229277</v>
       </c>
       <c r="M22" s="2">
         <f t="shared" si="0"/>
-        <v>1.0065477221894832</v>
+        <v>1.0045646069816763</v>
       </c>
       <c r="N22" s="2">
         <f t="shared" si="0"/>
@@ -2337,9 +2337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:T12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -2413,22 +2411,22 @@
         <v>19</v>
       </c>
       <c r="D2">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="E2" s="1">
-        <v>1.4641199999999999E-8</v>
+        <v>1.4162600000000001E-8</v>
       </c>
       <c r="F2">
-        <v>197.25</v>
+        <v>607.6</v>
       </c>
       <c r="G2">
-        <v>107.59</v>
+        <v>241.08</v>
       </c>
       <c r="H2">
-        <v>138.97999999999999</v>
+        <v>837.65</v>
       </c>
       <c r="I2">
-        <v>3.79</v>
+        <v>9.32</v>
       </c>
       <c r="J2">
         <v>6787</v>
@@ -2437,7 +2435,7 @@
         <v>6887</v>
       </c>
       <c r="L2">
-        <v>3036</v>
+        <v>3578</v>
       </c>
       <c r="M2">
         <v>549</v>
@@ -2472,19 +2470,19 @@
         <v>62</v>
       </c>
       <c r="E3" s="1">
-        <v>7.7051300000000003E-9</v>
+        <v>7.5683900000000006E-9</v>
       </c>
       <c r="F3">
-        <v>182.88</v>
+        <v>488.93</v>
       </c>
       <c r="G3">
-        <v>38.229999999999997</v>
+        <v>72.150000000000006</v>
       </c>
       <c r="H3">
-        <v>28</v>
+        <v>31.79</v>
       </c>
       <c r="I3">
-        <v>1.36</v>
+        <v>1.99</v>
       </c>
       <c r="J3">
         <v>4895</v>
@@ -2493,10 +2491,10 @@
         <v>5087</v>
       </c>
       <c r="L3">
-        <v>2276</v>
+        <v>2371</v>
       </c>
       <c r="M3">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="N3">
         <v>275</v>
@@ -2525,22 +2523,22 @@
         <v>19</v>
       </c>
       <c r="D4">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E4" s="1">
-        <v>3.5083799999999998E-9</v>
+        <v>3.44001E-9</v>
       </c>
       <c r="F4">
-        <v>41.95</v>
+        <v>160.72999999999999</v>
       </c>
       <c r="G4">
-        <v>3.26</v>
+        <v>6.42</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>5.05</v>
       </c>
       <c r="I4">
-        <v>0.17</v>
+        <v>0.31</v>
       </c>
       <c r="J4">
         <v>753</v>
@@ -2549,7 +2547,7 @@
         <v>883</v>
       </c>
       <c r="L4">
-        <v>408</v>
+        <v>446</v>
       </c>
       <c r="M4">
         <v>35</v>
@@ -2581,22 +2579,22 @@
         <v>19</v>
       </c>
       <c r="D5">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E5" s="1">
-        <v>1.9358099999999999E-8</v>
+        <v>1.9221399999999999E-8</v>
       </c>
       <c r="F5">
-        <v>4.68</v>
+        <v>13.19</v>
       </c>
       <c r="G5">
-        <v>4.5</v>
+        <v>8.4</v>
       </c>
       <c r="H5">
-        <v>18.05</v>
+        <v>32.35</v>
       </c>
       <c r="I5">
-        <v>1.04</v>
+        <v>1.74</v>
       </c>
       <c r="J5">
         <v>952</v>
@@ -2605,7 +2603,7 @@
         <v>889</v>
       </c>
       <c r="L5">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="M5">
         <v>32</v>
@@ -2637,22 +2635,22 @@
         <v>19</v>
       </c>
       <c r="D6">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E6" s="1">
-        <v>1.6727999999999999E-8</v>
+        <v>1.6864699999999999E-8</v>
       </c>
       <c r="F6">
-        <v>24.17</v>
+        <v>65.22</v>
       </c>
       <c r="G6">
-        <v>2.5</v>
+        <v>4.96</v>
       </c>
       <c r="H6">
-        <v>14.46</v>
+        <v>17.68</v>
       </c>
       <c r="I6">
-        <v>0.9</v>
+        <v>1.74</v>
       </c>
       <c r="J6">
         <v>603</v>
@@ -2661,7 +2659,7 @@
         <v>539</v>
       </c>
       <c r="L6">
-        <v>411</v>
+        <v>418</v>
       </c>
       <c r="M6">
         <v>20</v>
@@ -2693,22 +2691,22 @@
         <v>19</v>
       </c>
       <c r="D7">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E7" s="1">
-        <v>7.7310499999999993E-9</v>
+        <v>7.9361600000000004E-9</v>
       </c>
       <c r="F7">
-        <v>530.79999999999995</v>
+        <v>1213.79</v>
       </c>
       <c r="G7">
-        <v>114.24</v>
+        <v>226.77</v>
       </c>
       <c r="H7">
-        <v>1695.1</v>
+        <v>2755.01</v>
       </c>
       <c r="I7">
-        <v>19.02</v>
+        <v>28.24</v>
       </c>
       <c r="J7">
         <v>9917</v>
@@ -2717,10 +2715,10 @@
         <v>10470</v>
       </c>
       <c r="L7">
-        <v>5295</v>
+        <v>5438</v>
       </c>
       <c r="M7">
-        <v>431</v>
+        <v>438</v>
       </c>
       <c r="N7">
         <v>511</v>
@@ -2749,22 +2747,22 @@
         <v>19</v>
       </c>
       <c r="D8">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E8" s="1">
         <v>3.4799900000000001E-9</v>
       </c>
       <c r="F8">
-        <v>182.29</v>
+        <v>357.98</v>
       </c>
       <c r="G8">
-        <v>8.93</v>
+        <v>17.11</v>
       </c>
       <c r="H8">
-        <v>57.43</v>
+        <v>76.099999999999994</v>
       </c>
       <c r="I8">
-        <v>3.65</v>
+        <v>5.29</v>
       </c>
       <c r="J8">
         <v>1032</v>
@@ -2773,7 +2771,7 @@
         <v>1188</v>
       </c>
       <c r="L8">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="M8">
         <v>16</v>
@@ -2805,22 +2803,22 @@
         <v>19</v>
       </c>
       <c r="D9">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E9" s="1">
-        <v>7.8252099999999997E-9</v>
+        <v>7.8097300000000001E-9</v>
       </c>
       <c r="F9">
-        <v>143.13</v>
+        <v>329.46</v>
       </c>
       <c r="G9">
-        <v>23.6</v>
+        <v>45.22</v>
       </c>
       <c r="H9">
-        <v>38.19</v>
+        <v>79.86</v>
       </c>
       <c r="I9">
-        <v>1.29</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="J9">
         <v>3289</v>
@@ -2829,10 +2827,10 @@
         <v>3494</v>
       </c>
       <c r="L9">
-        <v>1577</v>
+        <v>1654</v>
       </c>
       <c r="M9">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="N9">
         <v>195</v>
@@ -2861,22 +2859,22 @@
         <v>19</v>
       </c>
       <c r="D10">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="E10" s="1">
-        <v>2.43587E-8</v>
+        <v>2.3880100000000002E-8</v>
       </c>
       <c r="F10">
-        <v>184.78</v>
+        <v>449.03</v>
       </c>
       <c r="G10">
-        <v>56.9</v>
+        <v>112.66</v>
       </c>
       <c r="H10">
-        <v>324.51</v>
+        <v>541.64</v>
       </c>
       <c r="I10">
-        <v>3.4</v>
+        <v>6.53</v>
       </c>
       <c r="J10">
         <v>4167</v>
@@ -2885,7 +2883,7 @@
         <v>4498</v>
       </c>
       <c r="L10">
-        <v>2612</v>
+        <v>2690</v>
       </c>
       <c r="M10">
         <v>254</v>
@@ -2923,16 +2921,16 @@
         <v>6.5730800000000002E-9</v>
       </c>
       <c r="F11">
-        <v>164.68</v>
+        <v>525.57000000000005</v>
       </c>
       <c r="G11">
-        <v>28.18</v>
+        <v>54.47</v>
       </c>
       <c r="H11">
-        <v>31.65</v>
+        <v>54.88</v>
       </c>
       <c r="I11">
-        <v>1.64</v>
+        <v>2.7</v>
       </c>
       <c r="J11">
         <v>4023</v>
@@ -2941,10 +2939,10 @@
         <v>4139</v>
       </c>
       <c r="L11">
-        <v>2069</v>
+        <v>2141</v>
       </c>
       <c r="M11">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="N11">
         <v>239</v>
@@ -2973,22 +2971,22 @@
         <v>19</v>
       </c>
       <c r="D12">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="E12" s="1">
-        <v>1.6312000000000001E-8</v>
+        <v>1.6106900000000001E-8</v>
       </c>
       <c r="F12">
-        <v>127.43</v>
+        <v>422.15</v>
       </c>
       <c r="G12">
-        <v>18.989999999999998</v>
+        <v>46.98</v>
       </c>
       <c r="H12">
-        <v>21.03</v>
+        <v>67.83</v>
       </c>
       <c r="I12">
-        <v>0.84</v>
+        <v>2.34</v>
       </c>
       <c r="J12">
         <v>3161</v>
@@ -2997,10 +2995,10 @@
         <v>3197</v>
       </c>
       <c r="L12">
-        <v>1348</v>
+        <v>1737</v>
       </c>
       <c r="M12">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N12">
         <v>38</v>

</xml_diff>